<commit_message>
Assigment 10 part 1
</commit_message>
<xml_diff>
--- a/student_courses.xlsx
+++ b/student_courses.xlsx
@@ -256,34 +256,34 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Bob Johnson</t>
+          <t>John Doe</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Data Structures</t>
+          <t>Introduction to Databases</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>A</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Bob Johnson</t>
+          <t>John Doe</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Data Structures</t>
+          <t>Web Development</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>B</t>
         </is>
       </c>
     </row>
@@ -341,51 +341,51 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Jane Smith</t>
+          <t>Bob Johnson</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Introduction to Databases</t>
+          <t>Data Structures</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>C</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Jane Smith</t>
+          <t>Bob Johnson</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Introduction to Databases</t>
+          <t>Data Structures</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>C</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Jane Smith</t>
+          <t>Bob Johnson</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Introduction to Databases</t>
+          <t>Data Structures</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>C</t>
         </is>
       </c>
     </row>
@@ -418,6 +418,74 @@
         </is>
       </c>
       <c r="C21" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>Jane Smith</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>Introduction to Databases</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>Jane Smith</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>Introduction to Databases</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>Jane Smith</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>Introduction to Databases</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>Jane Smith</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>Introduction to Databases</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
         <is>
           <t>A</t>
         </is>

</xml_diff>